<commit_message>
Set solver parameters to limit solve time to 60 seconds and enable search progress logging
</commit_message>
<xml_diff>
--- a/schedule_output.xlsx
+++ b/schedule_output.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C47"/>
+  <dimension ref="A1:D47"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -449,6 +449,11 @@
           <t>Assigned</t>
         </is>
       </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Drivers</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -463,7 +468,12 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Jaxon, Jack Mogelof, Paul, Alejandro Espinosa, Ali Awada</t>
+          <t>Paul, Blake Steel, Noah Yaffe</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Paul, Blake Steel, Noah Yaffe</t>
         </is>
       </c>
     </row>
@@ -480,7 +490,12 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Josh Greene, Henry, Matheo, Jamari Pitchford, George Ryckman, Jake Dieterich</t>
+          <t>Noah Yaffe, Harry Corbin</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Noah Yaffe, Harry Corbin</t>
         </is>
       </c>
     </row>
@@ -497,7 +512,12 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Jack Mogelof, Ben Kairouz, Alexander, Blake Steel, Noah Yaffe</t>
+          <t>Ezana, Blake Steel, Harry Corbin</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Blake Steel, Harry Corbin</t>
         </is>
       </c>
     </row>
@@ -514,7 +534,12 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Gabe Heller, Ben Kairouz, Ezana, Henry, Alejandro E. Ulvert, Adi</t>
+          <t>Alejandro E. Ulvert, Adi, Harry Corbin</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Alejandro E. Ulvert, Adi, Harry Corbin</t>
         </is>
       </c>
     </row>
@@ -531,7 +556,12 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Jaxon, Jack Mogelof, Paul, Alejandro Espinosa, Ali Awada</t>
+          <t>Paul, Blake Steel, Noah Yaffe</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Paul, Blake Steel, Noah Yaffe</t>
         </is>
       </c>
     </row>
@@ -548,7 +578,12 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Josh Greene, Henry, Matheo, Jamari Pitchford, George Ryckman, Jake Dieterich</t>
+          <t>Noah Yaffe, Harry Corbin</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>Noah Yaffe, Harry Corbin</t>
         </is>
       </c>
     </row>
@@ -565,7 +600,12 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Jaxon, Jack Mogelof, Gabe Heller, Ben Kairouz, Paul, Alexander, Josh Greene, Henry, Matheo, Alejandro Espinosa, Jamari Pitchford, Thor Waguespack, Edu, Ali Awada, George Ryckman, Jake Dieterich, Alejandro E. Ulvert, Adi, Blake Steel, Noah Yaffe</t>
+          <t>Alejandro E. Ulvert, Harry Corbin</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>Alejandro E. Ulvert, Harry Corbin</t>
         </is>
       </c>
     </row>
@@ -582,7 +622,12 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Jack Mogelof, Paul, Jake Dieterich, Blake Steel</t>
+          <t>George Ryckman, Jake Dieterich, Alejandro E. Ulvert</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>George Ryckman, Alejandro E. Ulvert</t>
         </is>
       </c>
     </row>
@@ -599,7 +644,12 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Jack Mogelof, Ezana, Alejandro L, Jamari Pitchford, Thor Waguespack, Edu, Alejandro E. Ulvert</t>
+          <t>Jake Dieterich, Adi</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>Adi</t>
         </is>
       </c>
     </row>
@@ -616,7 +666,12 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Kamsi, Ezana, Paul, Edu, Adi, Blake Steel</t>
+          <t>Paul, Edu, Ali Awada</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>Paul, Edu</t>
         </is>
       </c>
     </row>
@@ -633,7 +688,12 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Jack Mogelof, Paul, Jake Dieterich, Blake Steel</t>
+          <t>George Ryckman, Jake Dieterich, Alejandro E. Ulvert</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>George Ryckman, Alejandro E. Ulvert</t>
         </is>
       </c>
     </row>
@@ -650,7 +710,12 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Jack Mogelof, Ezana, Alejandro L, Jamari Pitchford, Thor Waguespack, Edu, Alejandro E. Ulvert</t>
+          <t>Jake Dieterich, Adi</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>Adi</t>
         </is>
       </c>
     </row>
@@ -667,7 +732,12 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Alejandro L, Harry Corbin</t>
+          <t>Ali Awada, George Ryckman</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>George Ryckman</t>
         </is>
       </c>
     </row>
@@ -684,7 +754,12 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Josh Greene, Henry, Noah Yaffe</t>
+          <t>Edu, George Ryckman, Blake Steel</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>Edu, George Ryckman, Blake Steel</t>
         </is>
       </c>
     </row>
@@ -701,7 +776,12 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Jaxon, Kamsi, Alejandro L</t>
+          <t>Henry, Jamari Pitchford</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>Jamari Pitchford</t>
         </is>
       </c>
     </row>
@@ -718,7 +798,12 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Gabe Heller, Ben Kairouz, Paul, Alexander, Jamari Pitchford, George Ryckman, Blake Steel, Harry Corbin</t>
+          <t>Thor Waguespack, Edu, Adi</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>Thor Waguespack, Edu, Adi</t>
         </is>
       </c>
     </row>
@@ -735,7 +820,12 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Alexander, Thor Waguespack, Adi</t>
+          <t>Ben Kairouz, Jamari Pitchford, Jake Dieterich</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>Ben Kairouz, Jamari Pitchford</t>
         </is>
       </c>
     </row>
@@ -752,7 +842,12 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Josh Greene, Henry, Noah Yaffe</t>
+          <t>Edu, George Ryckman, Blake Steel</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>Edu, George Ryckman, Blake Steel</t>
         </is>
       </c>
     </row>
@@ -769,7 +864,12 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Jaxon, Kamsi, Alejandro L</t>
+          <t>Henry, Jamari Pitchford</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>Jamari Pitchford</t>
         </is>
       </c>
     </row>
@@ -786,7 +886,12 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Jaxon, Jack Mogelof, Gabe Heller, Ben Kairouz, Kamsi, Ezana, Alexander, Josh Greene, Henry, Matheo, Alejandro Espinosa, Jamari Pitchford, Thor Waguespack, Edu, Ali Awada, George Ryckman, Jake Dieterich, Alejandro E. Ulvert, Adi, Blake Steel, Noah Yaffe</t>
+          <t>Matheo, Thor Waguespack</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>Matheo, Thor Waguespack</t>
         </is>
       </c>
     </row>
@@ -803,7 +908,12 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Kamsi, Alejandro L, Alejandro Espinosa, Edu, Alejandro E. Ulvert</t>
+          <t>Josh Greene, Matheo, Alejandro Espinosa</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>Josh Greene, Matheo, Alejandro Espinosa</t>
         </is>
       </c>
     </row>
@@ -820,7 +930,12 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Josh Greene, Henry, Thor Waguespack, Edu, Ali Awada, Harry Corbin</t>
+          <t>Jaxon, Matheo, Ali Awada</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>Jaxon, Matheo</t>
         </is>
       </c>
     </row>
@@ -837,7 +952,12 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Gabe Heller, Thor Waguespack, Adi, Harry Corbin</t>
+          <t>Paul, Thor Waguespack, Edu</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>Paul, Thor Waguespack, Edu</t>
         </is>
       </c>
     </row>
@@ -854,7 +974,12 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>Kamsi, Alejandro L, Alejandro Espinosa, Edu, Alejandro E. Ulvert</t>
+          <t>Josh Greene, Matheo, Alejandro Espinosa</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>Josh Greene, Matheo, Alejandro Espinosa</t>
         </is>
       </c>
     </row>
@@ -871,7 +996,12 @@
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>Josh Greene, Henry, Thor Waguespack, Edu, Ali Awada, Harry Corbin</t>
+          <t>Jaxon, Matheo, Ali Awada</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>Jaxon, Matheo</t>
         </is>
       </c>
     </row>
@@ -888,7 +1018,12 @@
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>Paul, Alejandro L</t>
+          <t>Alejandro Espinosa, Ali Awada</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>Alejandro Espinosa</t>
         </is>
       </c>
     </row>
@@ -905,7 +1040,12 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>Kamsi, George Ryckman, Noah Yaffe</t>
+          <t>Alexander, Alejandro L, Thor Waguespack</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>Alexander, Thor Waguespack</t>
         </is>
       </c>
     </row>
@@ -922,7 +1062,12 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>Jaxon, Ben Kairouz, Ezana</t>
+          <t>Ezana, Alexander</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>Alexander</t>
         </is>
       </c>
     </row>
@@ -939,7 +1084,12 @@
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>Gabe Heller, Ben Kairouz, Alexander, Alejandro Espinosa, Thor Waguespack, George Ryckman, Adi, Blake Steel, Harry Corbin</t>
+          <t>Henry, Jamari Pitchford, Adi</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>Jamari Pitchford, Adi</t>
         </is>
       </c>
     </row>
@@ -956,7 +1106,12 @@
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>Gabe Heller, Paul, Alexander, Alejandro L, Ali Awada, Alejandro E. Ulvert, Harry Corbin</t>
+          <t>Gabe Heller, Alejandro L, Alejandro Espinosa</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>Gabe Heller, Alejandro Espinosa</t>
         </is>
       </c>
     </row>
@@ -973,7 +1128,12 @@
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>Kamsi, George Ryckman, Noah Yaffe</t>
+          <t>Alexander, Alejandro L, Thor Waguespack</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>Alexander, Thor Waguespack</t>
         </is>
       </c>
     </row>
@@ -990,7 +1150,12 @@
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>Jaxon, Ben Kairouz, Ezana</t>
+          <t>Ezana, Alexander</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>Alexander</t>
         </is>
       </c>
     </row>
@@ -1007,7 +1172,12 @@
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>Jaxon, Jack Mogelof, Gabe Heller, Ben Kairouz, Kamsi, Ezana, Alexander, Josh Greene, Henry, Matheo, Alejandro Espinosa, Jamari Pitchford, Thor Waguespack, Edu, Ali Awada, George Ryckman, Jake Dieterich, Alejandro E. Ulvert, Adi, Blake Steel, Noah Yaffe, Harry Corbin</t>
+          <t>Paul, Henry</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>Paul</t>
         </is>
       </c>
     </row>
@@ -1024,7 +1194,12 @@
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>Jack Mogelof, Matheo, Jamari Pitchford</t>
+          <t>Jaxon, Josh Greene, Alejandro L</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>Jaxon, Josh Greene</t>
         </is>
       </c>
     </row>
@@ -1041,7 +1216,12 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>Ben Kairouz, Kamsi, Ezana, Ali Awada</t>
+          <t>Gabe Heller, Ezana</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>Gabe Heller</t>
         </is>
       </c>
     </row>
@@ -1058,7 +1238,12 @@
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>Gabe Heller, George Ryckman, Adi, Noah Yaffe, Harry Corbin</t>
+          <t>Jack Mogelof, Alexander, Henry</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>Jack Mogelof, Alexander</t>
         </is>
       </c>
     </row>
@@ -1075,7 +1260,12 @@
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>Ben Kairouz, Kamsi, Ezana, Paul, Alexander, Josh Greene, Henry, Matheo, Alejandro L, Jake Dieterich, Adi, Harry Corbin</t>
+          <t>Jaxon, Ben Kairouz, Josh Greene</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>Jaxon, Ben Kairouz, Josh Greene</t>
         </is>
       </c>
     </row>
@@ -1092,7 +1282,12 @@
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>Jack Mogelof, Matheo, Jamari Pitchford</t>
+          <t>Jaxon, Josh Greene, Alejandro L</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>Jaxon, Josh Greene</t>
         </is>
       </c>
     </row>
@@ -1109,7 +1304,12 @@
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>Ben Kairouz, Kamsi, Ezana, Ali Awada</t>
+          <t>Gabe Heller, Ezana</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>Gabe Heller</t>
         </is>
       </c>
     </row>
@@ -1126,7 +1326,12 @@
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>Paul, Alejandro L</t>
+          <t>Jack Mogelof, Ben Kairouz</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>Jack Mogelof, Ben Kairouz</t>
         </is>
       </c>
     </row>
@@ -1143,7 +1348,12 @@
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>Paul, Matheo, Alejandro Espinosa, Jake Dieterich</t>
+          <t>Gabe Heller, Ben Kairouz, Kamsi</t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>Gabe Heller, Ben Kairouz</t>
         </is>
       </c>
     </row>
@@ -1160,7 +1370,12 @@
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>Jaxon, Gabe Heller, Ezana, Alexander, Josh Greene, Henry, Matheo, Alejandro L, Alejandro Espinosa, Jamari Pitchford, Thor Waguespack, Edu, Ali Awada, George Ryckman, Jake Dieterich, Alejandro E. Ulvert, Adi, Blake Steel, Noah Yaffe, Harry Corbin</t>
+          <t>Jack Mogelof, Kamsi</t>
+        </is>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>Jack Mogelof</t>
         </is>
       </c>
     </row>
@@ -1177,7 +1392,12 @@
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>Jaxon, Gabe Heller, Kamsi, Alexander, Alejandro E. Ulvert, Blake Steel, Noah Yaffe</t>
+          <t>Jack Mogelof, Kamsi, Jamari Pitchford</t>
+        </is>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>Jack Mogelof, Jamari Pitchford</t>
         </is>
       </c>
     </row>
@@ -1194,7 +1414,12 @@
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>Paul, Matheo, Alejandro Espinosa, Jake Dieterich</t>
+          <t>Gabe Heller, Ben Kairouz, Kamsi</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>Gabe Heller, Ben Kairouz</t>
         </is>
       </c>
     </row>
@@ -1211,7 +1436,12 @@
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>Jaxon, Gabe Heller, Ezana, Alexander, Josh Greene, Henry, Matheo, Alejandro L, Alejandro Espinosa, Jamari Pitchford, Thor Waguespack, Edu, Ali Awada, George Ryckman, Jake Dieterich, Alejandro E. Ulvert, Adi, Blake Steel, Noah Yaffe, Harry Corbin</t>
+          <t>Jack Mogelof, Kamsi</t>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>Jack Mogelof</t>
         </is>
       </c>
     </row>
@@ -1228,7 +1458,12 @@
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>Jaxon, Jack Mogelof, Gabe Heller, Ben Kairouz, Alexander, Josh Greene, Matheo, Alejandro Espinosa, Jamari Pitchford, Thor Waguespack, Edu, Ali Awada, George Ryckman, Jake Dieterich, Alejandro E. Ulvert, Adi, Blake Steel, Noah Yaffe, Harry Corbin</t>
+          <t>Alejandro Espinosa, Noah Yaffe</t>
+        </is>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>Alejandro Espinosa, Noah Yaffe</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Refactor shift scheduling logic to enhance shift instance handling, implement maximum staffing constraints, and ensure fairness in shift assignments.
</commit_message>
<xml_diff>
--- a/schedule_output.xlsx
+++ b/schedule_output.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D47"/>
+  <dimension ref="A1:E47"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,10 +446,15 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
+          <t>Instance</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
           <t>Assigned</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>Drivers</t>
         </is>
@@ -466,14 +471,17 @@
           <t>8-11</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>Paul, Blake Steel, Noah Yaffe</t>
-        </is>
+      <c r="C2" t="n">
+        <v>0</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Paul, Blake Steel, Noah Yaffe</t>
+          <t>Paul, Matheo, Thor Waguespack</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>Paul, Matheo, Thor Waguespack</t>
         </is>
       </c>
     </row>
@@ -488,14 +496,17 @@
           <t>11-2</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>Noah Yaffe, Harry Corbin</t>
-        </is>
+      <c r="C3" t="n">
+        <v>1</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Noah Yaffe, Harry Corbin</t>
+          <t>Matheo, Blake Steel</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Matheo, Blake Steel</t>
         </is>
       </c>
     </row>
@@ -510,14 +521,17 @@
           <t>2-5</t>
         </is>
       </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>Ezana, Blake Steel, Harry Corbin</t>
-        </is>
+      <c r="C4" t="n">
+        <v>2</v>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Blake Steel, Harry Corbin</t>
+          <t>Kamsi, Blake Steel, Noah Yaffe</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Blake Steel, Noah Yaffe</t>
         </is>
       </c>
     </row>
@@ -532,14 +546,17 @@
           <t>5-8</t>
         </is>
       </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>Alejandro E. Ulvert, Adi, Harry Corbin</t>
-        </is>
+      <c r="C5" t="n">
+        <v>3</v>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Alejandro E. Ulvert, Adi, Harry Corbin</t>
+          <t>Jack Mogelof, Alejandro L, Jamari Pitchford</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Jack Mogelof, Jamari Pitchford</t>
         </is>
       </c>
     </row>
@@ -554,14 +571,17 @@
           <t>8-11</t>
         </is>
       </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>Paul, Blake Steel, Noah Yaffe</t>
-        </is>
+      <c r="C6" t="n">
+        <v>4</v>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Paul, Blake Steel, Noah Yaffe</t>
+          <t>Ali Awada, Alejandro E. Ulvert, Harry Corbin</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>Alejandro E. Ulvert, Harry Corbin</t>
         </is>
       </c>
     </row>
@@ -576,14 +596,17 @@
           <t>11-2</t>
         </is>
       </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>Noah Yaffe, Harry Corbin</t>
-        </is>
+      <c r="C7" t="n">
+        <v>5</v>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Noah Yaffe, Harry Corbin</t>
+          <t>Kamsi, Jamari Pitchford</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>Jamari Pitchford</t>
         </is>
       </c>
     </row>
@@ -598,14 +621,17 @@
           <t>2-8 (Night)</t>
         </is>
       </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>Alejandro E. Ulvert, Harry Corbin</t>
-        </is>
+      <c r="C8" t="n">
+        <v>6</v>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Alejandro E. Ulvert, Harry Corbin</t>
+          <t>Jake Dieterich, Alejandro E. Ulvert</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>Alejandro E. Ulvert</t>
         </is>
       </c>
     </row>
@@ -620,14 +646,17 @@
           <t>8-11</t>
         </is>
       </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>George Ryckman, Jake Dieterich, Alejandro E. Ulvert</t>
-        </is>
+      <c r="C9" t="n">
+        <v>0</v>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>George Ryckman, Alejandro E. Ulvert</t>
+          <t>Kamsi, Edu, Adi</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>Edu, Adi</t>
         </is>
       </c>
     </row>
@@ -642,14 +671,17 @@
           <t>11-2</t>
         </is>
       </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>Jake Dieterich, Adi</t>
-        </is>
+      <c r="C10" t="n">
+        <v>1</v>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Adi</t>
+          <t>Matheo, Noah Yaffe</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>Matheo, Noah Yaffe</t>
         </is>
       </c>
     </row>
@@ -664,14 +696,17 @@
           <t>2-5</t>
         </is>
       </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>Paul, Edu, Ali Awada</t>
-        </is>
+      <c r="C11" t="n">
+        <v>2</v>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Paul, Edu</t>
+          <t>Alexander, Alejandro L, George Ryckman</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>Alexander, George Ryckman</t>
         </is>
       </c>
     </row>
@@ -686,14 +721,17 @@
           <t>8-11</t>
         </is>
       </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>George Ryckman, Jake Dieterich, Alejandro E. Ulvert</t>
-        </is>
+      <c r="C12" t="n">
+        <v>3</v>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>George Ryckman, Alejandro E. Ulvert</t>
+          <t>Jaxon, Kamsi, George Ryckman</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>Jaxon, George Ryckman</t>
         </is>
       </c>
     </row>
@@ -708,14 +746,17 @@
           <t>11-2</t>
         </is>
       </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>Jake Dieterich, Adi</t>
-        </is>
+      <c r="C13" t="n">
+        <v>4</v>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>Adi</t>
+          <t>Jamari Pitchford, Edu</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>Jamari Pitchford, Edu</t>
         </is>
       </c>
     </row>
@@ -730,14 +771,17 @@
           <t>2-8 (Night)</t>
         </is>
       </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>Ali Awada, George Ryckman</t>
-        </is>
+      <c r="C14" t="n">
+        <v>5</v>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>George Ryckman</t>
+          <t>Matheo, Alejandro Espinosa</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>Matheo, Alejandro Espinosa</t>
         </is>
       </c>
     </row>
@@ -752,14 +796,17 @@
           <t>8-11</t>
         </is>
       </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>Edu, George Ryckman, Blake Steel</t>
-        </is>
+      <c r="C15" t="n">
+        <v>0</v>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>Edu, George Ryckman, Blake Steel</t>
+          <t>Josh Greene, Alejandro Espinosa, Jamari Pitchford</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>Josh Greene, Alejandro Espinosa, Jamari Pitchford</t>
         </is>
       </c>
     </row>
@@ -774,14 +821,17 @@
           <t>11-2</t>
         </is>
       </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>Henry, Jamari Pitchford</t>
-        </is>
+      <c r="C16" t="n">
+        <v>1</v>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>Jamari Pitchford</t>
+          <t>Thor Waguespack, Ali Awada</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>Thor Waguespack</t>
         </is>
       </c>
     </row>
@@ -796,14 +846,17 @@
           <t>2-5</t>
         </is>
       </c>
-      <c r="C17" t="inlineStr">
-        <is>
-          <t>Thor Waguespack, Edu, Adi</t>
-        </is>
+      <c r="C17" t="n">
+        <v>2</v>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>Thor Waguespack, Edu, Adi</t>
+          <t>Jack Mogelof, Alejandro L, Adi</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>Jack Mogelof, Adi</t>
         </is>
       </c>
     </row>
@@ -818,14 +871,17 @@
           <t>5-8</t>
         </is>
       </c>
-      <c r="C18" t="inlineStr">
-        <is>
-          <t>Ben Kairouz, Jamari Pitchford, Jake Dieterich</t>
-        </is>
+      <c r="C18" t="n">
+        <v>3</v>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>Ben Kairouz, Jamari Pitchford</t>
+          <t>Gabe Heller, Alejandro L, Adi</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>Gabe Heller, Adi</t>
         </is>
       </c>
     </row>
@@ -840,14 +896,17 @@
           <t>8-11</t>
         </is>
       </c>
-      <c r="C19" t="inlineStr">
-        <is>
-          <t>Edu, George Ryckman, Blake Steel</t>
-        </is>
+      <c r="C19" t="n">
+        <v>4</v>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>Edu, George Ryckman, Blake Steel</t>
+          <t>Gabe Heller, Jake Dieterich, Blake Steel</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>Gabe Heller, Blake Steel</t>
         </is>
       </c>
     </row>
@@ -862,14 +921,17 @@
           <t>11-2</t>
         </is>
       </c>
-      <c r="C20" t="inlineStr">
-        <is>
-          <t>Henry, Jamari Pitchford</t>
-        </is>
+      <c r="C20" t="n">
+        <v>5</v>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>Jamari Pitchford</t>
+          <t>Paul, Henry, Harry Corbin</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>Paul, Harry Corbin</t>
         </is>
       </c>
     </row>
@@ -884,14 +946,17 @@
           <t>2-8 (Night)</t>
         </is>
       </c>
-      <c r="C21" t="inlineStr">
-        <is>
-          <t>Matheo, Thor Waguespack</t>
-        </is>
+      <c r="C21" t="n">
+        <v>6</v>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>Matheo, Thor Waguespack</t>
+          <t>Ezana, Edu</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>Edu</t>
         </is>
       </c>
     </row>
@@ -906,14 +971,17 @@
           <t>8-11</t>
         </is>
       </c>
-      <c r="C22" t="inlineStr">
-        <is>
-          <t>Josh Greene, Matheo, Alejandro Espinosa</t>
-        </is>
+      <c r="C22" t="n">
+        <v>0</v>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>Josh Greene, Matheo, Alejandro Espinosa</t>
+          <t>Paul, Josh Greene, George Ryckman</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>Paul, Josh Greene, George Ryckman</t>
         </is>
       </c>
     </row>
@@ -928,14 +996,17 @@
           <t>11-2</t>
         </is>
       </c>
-      <c r="C23" t="inlineStr">
-        <is>
-          <t>Jaxon, Matheo, Ali Awada</t>
-        </is>
+      <c r="C23" t="n">
+        <v>1</v>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>Jaxon, Matheo</t>
+          <t>Alejandro Espinosa, Thor Waguespack</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>Alejandro Espinosa, Thor Waguespack</t>
         </is>
       </c>
     </row>
@@ -950,14 +1021,17 @@
           <t>2-5</t>
         </is>
       </c>
-      <c r="C24" t="inlineStr">
-        <is>
-          <t>Paul, Thor Waguespack, Edu</t>
-        </is>
+      <c r="C24" t="n">
+        <v>2</v>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>Paul, Thor Waguespack, Edu</t>
+          <t>Henry, Adi, Noah Yaffe</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>Adi, Noah Yaffe</t>
         </is>
       </c>
     </row>
@@ -972,14 +1046,17 @@
           <t>8-11</t>
         </is>
       </c>
-      <c r="C25" t="inlineStr">
-        <is>
-          <t>Josh Greene, Matheo, Alejandro Espinosa</t>
-        </is>
+      <c r="C25" t="n">
+        <v>3</v>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>Josh Greene, Matheo, Alejandro Espinosa</t>
+          <t>Ben Kairouz, Alejandro Espinosa, Alejandro E. Ulvert</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>Ben Kairouz, Alejandro Espinosa, Alejandro E. Ulvert</t>
         </is>
       </c>
     </row>
@@ -994,14 +1071,17 @@
           <t>11-2</t>
         </is>
       </c>
-      <c r="C26" t="inlineStr">
-        <is>
-          <t>Jaxon, Matheo, Ali Awada</t>
-        </is>
+      <c r="C26" t="n">
+        <v>4</v>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>Jaxon, Matheo</t>
+          <t>Gabe Heller, Alexander, Ali Awada</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>Gabe Heller, Alexander</t>
         </is>
       </c>
     </row>
@@ -1016,14 +1096,17 @@
           <t>2-8 (Night)</t>
         </is>
       </c>
-      <c r="C27" t="inlineStr">
-        <is>
-          <t>Alejandro Espinosa, Ali Awada</t>
-        </is>
+      <c r="C27" t="n">
+        <v>5</v>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>Alejandro Espinosa</t>
+          <t>Jack Mogelof, Jake Dieterich</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>Jack Mogelof</t>
         </is>
       </c>
     </row>
@@ -1038,14 +1121,17 @@
           <t>8-11</t>
         </is>
       </c>
-      <c r="C28" t="inlineStr">
-        <is>
-          <t>Alexander, Alejandro L, Thor Waguespack</t>
-        </is>
+      <c r="C28" t="n">
+        <v>0</v>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>Alexander, Thor Waguespack</t>
+          <t>Thor Waguespack, Alejandro E. Ulvert, Noah Yaffe</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>Thor Waguespack, Alejandro E. Ulvert, Noah Yaffe</t>
         </is>
       </c>
     </row>
@@ -1060,14 +1146,17 @@
           <t>11-2</t>
         </is>
       </c>
-      <c r="C29" t="inlineStr">
-        <is>
-          <t>Ezana, Alexander</t>
-        </is>
+      <c r="C29" t="n">
+        <v>1</v>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>Alexander</t>
+          <t>Jack Mogelof, Ali Awada</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>Jack Mogelof</t>
         </is>
       </c>
     </row>
@@ -1082,14 +1171,17 @@
           <t>2-5</t>
         </is>
       </c>
-      <c r="C30" t="inlineStr">
-        <is>
-          <t>Henry, Jamari Pitchford, Adi</t>
-        </is>
+      <c r="C30" t="n">
+        <v>2</v>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>Jamari Pitchford, Adi</t>
+          <t>Josh Greene, Henry, Adi</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>Josh Greene, Adi</t>
         </is>
       </c>
     </row>
@@ -1104,14 +1196,17 @@
           <t>5-8</t>
         </is>
       </c>
-      <c r="C31" t="inlineStr">
-        <is>
-          <t>Gabe Heller, Alejandro L, Alejandro Espinosa</t>
-        </is>
+      <c r="C31" t="n">
+        <v>3</v>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>Gabe Heller, Alejandro Espinosa</t>
+          <t>Thor Waguespack, Blake Steel, Harry Corbin</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>Thor Waguespack, Blake Steel, Harry Corbin</t>
         </is>
       </c>
     </row>
@@ -1126,14 +1221,17 @@
           <t>8-11</t>
         </is>
       </c>
-      <c r="C32" t="inlineStr">
-        <is>
-          <t>Alexander, Alejandro L, Thor Waguespack</t>
-        </is>
+      <c r="C32" t="n">
+        <v>4</v>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>Alexander, Thor Waguespack</t>
+          <t>Josh Greene, Henry, George Ryckman</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>Josh Greene, George Ryckman</t>
         </is>
       </c>
     </row>
@@ -1148,14 +1246,17 @@
           <t>11-2</t>
         </is>
       </c>
-      <c r="C33" t="inlineStr">
-        <is>
-          <t>Ezana, Alexander</t>
-        </is>
+      <c r="C33" t="n">
+        <v>5</v>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>Alexander</t>
+          <t>Alexander, Edu</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>Alexander, Edu</t>
         </is>
       </c>
     </row>
@@ -1170,14 +1271,17 @@
           <t>2-8 (Night)</t>
         </is>
       </c>
-      <c r="C34" t="inlineStr">
-        <is>
-          <t>Paul, Henry</t>
-        </is>
+      <c r="C34" t="n">
+        <v>6</v>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>Paul</t>
+          <t>Jaxon, Alejandro Espinosa</t>
+        </is>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>Jaxon, Alejandro Espinosa</t>
         </is>
       </c>
     </row>
@@ -1192,14 +1296,17 @@
           <t>8-11</t>
         </is>
       </c>
-      <c r="C35" t="inlineStr">
-        <is>
-          <t>Jaxon, Josh Greene, Alejandro L</t>
-        </is>
+      <c r="C35" t="n">
+        <v>0</v>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>Jaxon, Josh Greene</t>
+          <t>Gabe Heller, Ezana, Harry Corbin</t>
+        </is>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>Gabe Heller, Harry Corbin</t>
         </is>
       </c>
     </row>
@@ -1214,14 +1321,17 @@
           <t>11-2</t>
         </is>
       </c>
-      <c r="C36" t="inlineStr">
-        <is>
-          <t>Gabe Heller, Ezana</t>
-        </is>
+      <c r="C36" t="n">
+        <v>1</v>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>Gabe Heller</t>
+          <t>Jaxon, Ezana, Ali Awada</t>
+        </is>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>Jaxon</t>
         </is>
       </c>
     </row>
@@ -1236,14 +1346,17 @@
           <t>2-5</t>
         </is>
       </c>
-      <c r="C37" t="inlineStr">
-        <is>
-          <t>Jack Mogelof, Alexander, Henry</t>
-        </is>
+      <c r="C37" t="n">
+        <v>2</v>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>Jack Mogelof, Alexander</t>
+          <t>Jaxon, Gabe Heller, Alexander</t>
+        </is>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>Jaxon, Gabe Heller, Alexander</t>
         </is>
       </c>
     </row>
@@ -1258,14 +1371,17 @@
           <t>5-8</t>
         </is>
       </c>
-      <c r="C38" t="inlineStr">
-        <is>
-          <t>Jaxon, Ben Kairouz, Josh Greene</t>
-        </is>
+      <c r="C38" t="n">
+        <v>3</v>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>Jaxon, Ben Kairouz, Josh Greene</t>
+          <t>Ben Kairouz, Alexander, Harry Corbin</t>
+        </is>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>Ben Kairouz, Alexander, Harry Corbin</t>
         </is>
       </c>
     </row>
@@ -1280,14 +1396,17 @@
           <t>8-11</t>
         </is>
       </c>
-      <c r="C39" t="inlineStr">
-        <is>
-          <t>Jaxon, Josh Greene, Alejandro L</t>
-        </is>
+      <c r="C39" t="n">
+        <v>4</v>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>Jaxon, Josh Greene</t>
+          <t>Alejandro L, George Ryckman, Blake Steel</t>
+        </is>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>George Ryckman, Blake Steel</t>
         </is>
       </c>
     </row>
@@ -1302,14 +1421,17 @@
           <t>11-2</t>
         </is>
       </c>
-      <c r="C40" t="inlineStr">
-        <is>
-          <t>Gabe Heller, Ezana</t>
-        </is>
+      <c r="C40" t="n">
+        <v>5</v>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>Gabe Heller</t>
+          <t>Ezana, Edu</t>
+        </is>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>Edu</t>
         </is>
       </c>
     </row>
@@ -1324,14 +1446,17 @@
           <t>2-8 (Night)</t>
         </is>
       </c>
-      <c r="C41" t="inlineStr">
-        <is>
-          <t>Jack Mogelof, Ben Kairouz</t>
-        </is>
+      <c r="C41" t="n">
+        <v>6</v>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>Jack Mogelof, Ben Kairouz</t>
+          <t>Henry, Jamari Pitchford</t>
+        </is>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>Jamari Pitchford</t>
         </is>
       </c>
     </row>
@@ -1346,14 +1471,17 @@
           <t>8-11</t>
         </is>
       </c>
-      <c r="C42" t="inlineStr">
-        <is>
-          <t>Gabe Heller, Ben Kairouz, Kamsi</t>
-        </is>
+      <c r="C42" t="n">
+        <v>0</v>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>Gabe Heller, Ben Kairouz</t>
+          <t>Ben Kairouz, Kamsi, Paul</t>
+        </is>
+      </c>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>Ben Kairouz, Paul</t>
         </is>
       </c>
     </row>
@@ -1368,14 +1496,17 @@
           <t>11-2</t>
         </is>
       </c>
-      <c r="C43" t="inlineStr">
-        <is>
-          <t>Jack Mogelof, Kamsi</t>
-        </is>
+      <c r="C43" t="n">
+        <v>1</v>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>Jack Mogelof</t>
+          <t>Jaxon, Jake Dieterich</t>
+        </is>
+      </c>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>Jaxon</t>
         </is>
       </c>
     </row>
@@ -1390,14 +1521,17 @@
           <t>2-5</t>
         </is>
       </c>
-      <c r="C44" t="inlineStr">
-        <is>
-          <t>Jack Mogelof, Kamsi, Jamari Pitchford</t>
-        </is>
+      <c r="C44" t="n">
+        <v>2</v>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>Jack Mogelof, Jamari Pitchford</t>
+          <t>Jack Mogelof, Josh Greene, Jake Dieterich</t>
+        </is>
+      </c>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>Jack Mogelof, Josh Greene</t>
         </is>
       </c>
     </row>
@@ -1412,14 +1546,17 @@
           <t>8-11</t>
         </is>
       </c>
-      <c r="C45" t="inlineStr">
-        <is>
-          <t>Gabe Heller, Ben Kairouz, Kamsi</t>
-        </is>
+      <c r="C45" t="n">
+        <v>3</v>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>Gabe Heller, Ben Kairouz</t>
+          <t>Paul, Matheo, Noah Yaffe</t>
+        </is>
+      </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>Paul, Matheo, Noah Yaffe</t>
         </is>
       </c>
     </row>
@@ -1434,14 +1571,17 @@
           <t>11-2</t>
         </is>
       </c>
-      <c r="C46" t="inlineStr">
-        <is>
-          <t>Jack Mogelof, Kamsi</t>
-        </is>
+      <c r="C46" t="n">
+        <v>4</v>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>Jack Mogelof</t>
+          <t>Ben Kairouz, Ezana</t>
+        </is>
+      </c>
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>Ben Kairouz</t>
         </is>
       </c>
     </row>
@@ -1456,14 +1596,17 @@
           <t>2-8 (Night)</t>
         </is>
       </c>
-      <c r="C47" t="inlineStr">
-        <is>
-          <t>Alejandro Espinosa, Noah Yaffe</t>
-        </is>
+      <c r="C47" t="n">
+        <v>5</v>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>Alejandro Espinosa, Noah Yaffe</t>
+          <t>Ben Kairouz, Alejandro E. Ulvert</t>
+        </is>
+      </c>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>Ben Kairouz, Alejandro E. Ulvert</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Add CSV conversion utility and enhance scheduling conflict detection
</commit_message>
<xml_diff>
--- a/schedule_output.xlsx
+++ b/schedule_output.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E47"/>
+  <dimension ref="A1:E50"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -468,7 +468,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>8-11</t>
+          <t>08:00-11:00</t>
         </is>
       </c>
       <c r="C2" t="n">
@@ -476,12 +476,12 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Paul, Matheo, Thor Waguespack</t>
+          <t>Alexander, Alejandro L, Adi</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Paul, Matheo, Thor Waguespack</t>
+          <t>Alexander, Adi</t>
         </is>
       </c>
     </row>
@@ -493,7 +493,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>11-2</t>
+          <t>11:00-14:00</t>
         </is>
       </c>
       <c r="C3" t="n">
@@ -501,12 +501,12 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Matheo, Blake Steel</t>
+          <t>Jaxon, Ben Kairouz, Kamsi</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Matheo, Blake Steel</t>
+          <t>Jaxon, Ben Kairouz</t>
         </is>
       </c>
     </row>
@@ -518,7 +518,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>2-5</t>
+          <t>14:00-17:00</t>
         </is>
       </c>
       <c r="C4" t="n">
@@ -526,12 +526,12 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Kamsi, Blake Steel, Noah Yaffe</t>
+          <t>Henry, Jamari Pitchford, Harry Corbin</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Blake Steel, Noah Yaffe</t>
+          <t>Jamari Pitchford, Harry Corbin</t>
         </is>
       </c>
     </row>
@@ -543,7 +543,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>5-8</t>
+          <t>17:00-20:00</t>
         </is>
       </c>
       <c r="C5" t="n">
@@ -551,12 +551,12 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Jack Mogelof, Alejandro L, Jamari Pitchford</t>
+          <t>Thor Waguespack, Ali Awada, Alejandro E. Ulvert</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Jack Mogelof, Jamari Pitchford</t>
+          <t>Thor Waguespack, Alejandro E. Ulvert</t>
         </is>
       </c>
     </row>
@@ -568,22 +568,14 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>8-11</t>
+          <t>20:00-23:00</t>
         </is>
       </c>
       <c r="C6" t="n">
         <v>4</v>
       </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>Ali Awada, Alejandro E. Ulvert, Harry Corbin</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>Alejandro E. Ulvert, Harry Corbin</t>
-        </is>
-      </c>
+      <c r="D6" t="inlineStr"/>
+      <c r="E6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -593,22 +585,14 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>11-2</t>
+          <t>23:00-02:00</t>
         </is>
       </c>
       <c r="C7" t="n">
         <v>5</v>
       </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>Kamsi, Jamari Pitchford</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>Jamari Pitchford</t>
-        </is>
-      </c>
+      <c r="D7" t="inlineStr"/>
+      <c r="E7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -618,7 +602,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>2-8 (Night)</t>
+          <t>02:00-08:00 (Night)</t>
         </is>
       </c>
       <c r="C8" t="n">
@@ -626,12 +610,12 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Jake Dieterich, Alejandro E. Ulvert</t>
+          <t>Ezana, Paul</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>Alejandro E. Ulvert</t>
+          <t>Paul</t>
         </is>
       </c>
     </row>
@@ -643,7 +627,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>8-11</t>
+          <t>08:00-11:00</t>
         </is>
       </c>
       <c r="C9" t="n">
@@ -651,12 +635,12 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Kamsi, Edu, Adi</t>
+          <t>Paul, Alexander, George Ryckman</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>Edu, Adi</t>
+          <t>Paul, Alexander, George Ryckman</t>
         </is>
       </c>
     </row>
@@ -668,7 +652,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>11-2</t>
+          <t>11:00-14:00</t>
         </is>
       </c>
       <c r="C10" t="n">
@@ -676,12 +660,12 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Matheo, Noah Yaffe</t>
+          <t>Alejandro Espinosa, Jamari Pitchford, Blake Steel</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>Matheo, Noah Yaffe</t>
+          <t>Alejandro Espinosa, Jamari Pitchford, Blake Steel</t>
         </is>
       </c>
     </row>
@@ -693,7 +677,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>2-5</t>
+          <t>14:00-17:00</t>
         </is>
       </c>
       <c r="C11" t="n">
@@ -701,12 +685,12 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Alexander, Alejandro L, George Ryckman</t>
+          <t>Josh Greene, Matheo, Jake Dieterich</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>Alexander, George Ryckman</t>
+          <t>Josh Greene, Matheo</t>
         </is>
       </c>
     </row>
@@ -718,7 +702,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>8-11</t>
+          <t>17:00-20:00</t>
         </is>
       </c>
       <c r="C12" t="n">
@@ -726,12 +710,12 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>Jaxon, Kamsi, George Ryckman</t>
+          <t>Jaxon, Gabe Heller, Alejandro E. Ulvert</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>Jaxon, George Ryckman</t>
+          <t>Jaxon, Gabe Heller, Alejandro E. Ulvert</t>
         </is>
       </c>
     </row>
@@ -743,22 +727,14 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>11-2</t>
+          <t>20:00-23:00</t>
         </is>
       </c>
       <c r="C13" t="n">
         <v>4</v>
       </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>Jamari Pitchford, Edu</t>
-        </is>
-      </c>
-      <c r="E13" t="inlineStr">
-        <is>
-          <t>Jamari Pitchford, Edu</t>
-        </is>
-      </c>
+      <c r="D13" t="inlineStr"/>
+      <c r="E13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -768,45 +744,37 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>2-8 (Night)</t>
+          <t>23:00-02:00</t>
         </is>
       </c>
       <c r="C14" t="n">
         <v>5</v>
       </c>
-      <c r="D14" t="inlineStr">
-        <is>
-          <t>Matheo, Alejandro Espinosa</t>
-        </is>
-      </c>
-      <c r="E14" t="inlineStr">
-        <is>
-          <t>Matheo, Alejandro Espinosa</t>
-        </is>
-      </c>
+      <c r="D14" t="inlineStr"/>
+      <c r="E14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Wednesday</t>
+          <t>Tuesday</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>8-11</t>
+          <t>02:00-08:00 (Night)</t>
         </is>
       </c>
       <c r="C15" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>Josh Greene, Alejandro Espinosa, Jamari Pitchford</t>
+          <t>Jack Mogelof, Henry</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>Josh Greene, Alejandro Espinosa, Jamari Pitchford</t>
+          <t>Jack Mogelof</t>
         </is>
       </c>
     </row>
@@ -818,20 +786,20 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>11-2</t>
+          <t>08:00-11:00</t>
         </is>
       </c>
       <c r="C16" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>Thor Waguespack, Ali Awada</t>
+          <t>Ezana, Josh Greene, Thor Waguespack</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>Thor Waguespack</t>
+          <t>Josh Greene, Thor Waguespack</t>
         </is>
       </c>
     </row>
@@ -843,20 +811,20 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>2-5</t>
+          <t>11:00-14:00</t>
         </is>
       </c>
       <c r="C17" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>Jack Mogelof, Alejandro L, Adi</t>
+          <t>Gabe Heller, Jake Dieterich, Noah Yaffe</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>Jack Mogelof, Adi</t>
+          <t>Gabe Heller, Noah Yaffe</t>
         </is>
       </c>
     </row>
@@ -868,20 +836,20 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>5-8</t>
+          <t>14:00-17:00</t>
         </is>
       </c>
       <c r="C18" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>Gabe Heller, Alejandro L, Adi</t>
+          <t>Henry, Alejandro Espinosa, Edu</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>Gabe Heller, Adi</t>
+          <t>Alejandro Espinosa, Edu</t>
         </is>
       </c>
     </row>
@@ -893,20 +861,20 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>8-11</t>
+          <t>17:00-20:00</t>
         </is>
       </c>
       <c r="C19" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>Gabe Heller, Jake Dieterich, Blake Steel</t>
+          <t>Ben Kairouz, Kamsi, Harry Corbin</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>Gabe Heller, Blake Steel</t>
+          <t>Ben Kairouz, Harry Corbin</t>
         </is>
       </c>
     </row>
@@ -918,22 +886,14 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>11-2</t>
+          <t>20:00-23:00</t>
         </is>
       </c>
       <c r="C20" t="n">
-        <v>5</v>
-      </c>
-      <c r="D20" t="inlineStr">
-        <is>
-          <t>Paul, Henry, Harry Corbin</t>
-        </is>
-      </c>
-      <c r="E20" t="inlineStr">
-        <is>
-          <t>Paul, Harry Corbin</t>
-        </is>
-      </c>
+        <v>4</v>
+      </c>
+      <c r="D20" t="inlineStr"/>
+      <c r="E20" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -943,45 +903,37 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>2-8 (Night)</t>
+          <t>23:00-02:00</t>
         </is>
       </c>
       <c r="C21" t="n">
-        <v>6</v>
-      </c>
-      <c r="D21" t="inlineStr">
-        <is>
-          <t>Ezana, Edu</t>
-        </is>
-      </c>
-      <c r="E21" t="inlineStr">
-        <is>
-          <t>Edu</t>
-        </is>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="D21" t="inlineStr"/>
+      <c r="E21" t="inlineStr"/>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Thursday</t>
+          <t>Wednesday</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>8-11</t>
+          <t>02:00-08:00 (Night)</t>
         </is>
       </c>
       <c r="C22" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>Paul, Josh Greene, George Ryckman</t>
+          <t>Ali Awada, Blake Steel</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>Paul, Josh Greene, George Ryckman</t>
+          <t>Blake Steel</t>
         </is>
       </c>
     </row>
@@ -993,20 +945,20 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>11-2</t>
+          <t>08:00-11:00</t>
         </is>
       </c>
       <c r="C23" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>Alejandro Espinosa, Thor Waguespack</t>
+          <t>Jack Mogelof, George Ryckman, Noah Yaffe</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>Alejandro Espinosa, Thor Waguespack</t>
+          <t>Jack Mogelof, George Ryckman, Noah Yaffe</t>
         </is>
       </c>
     </row>
@@ -1018,20 +970,20 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>2-5</t>
+          <t>11:00-14:00</t>
         </is>
       </c>
       <c r="C24" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>Henry, Adi, Noah Yaffe</t>
+          <t>Ezana, Josh Greene, Thor Waguespack</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>Adi, Noah Yaffe</t>
+          <t>Josh Greene, Thor Waguespack</t>
         </is>
       </c>
     </row>
@@ -1043,20 +995,20 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>8-11</t>
+          <t>14:00-17:00</t>
         </is>
       </c>
       <c r="C25" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>Ben Kairouz, Alejandro Espinosa, Alejandro E. Ulvert</t>
+          <t>Gabe Heller, Ali Awada, Alejandro E. Ulvert</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>Ben Kairouz, Alejandro Espinosa, Alejandro E. Ulvert</t>
+          <t>Gabe Heller, Alejandro E. Ulvert</t>
         </is>
       </c>
     </row>
@@ -1068,20 +1020,20 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>11-2</t>
+          <t>17:00-20:00</t>
         </is>
       </c>
       <c r="C26" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>Gabe Heller, Alexander, Ali Awada</t>
+          <t>Matheo, Edu, Adi</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>Gabe Heller, Alexander</t>
+          <t>Matheo, Edu, Adi</t>
         </is>
       </c>
     </row>
@@ -1093,70 +1045,54 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>2-8 (Night)</t>
+          <t>20:00-23:00</t>
         </is>
       </c>
       <c r="C27" t="n">
-        <v>5</v>
-      </c>
-      <c r="D27" t="inlineStr">
-        <is>
-          <t>Jack Mogelof, Jake Dieterich</t>
-        </is>
-      </c>
-      <c r="E27" t="inlineStr">
-        <is>
-          <t>Jack Mogelof</t>
-        </is>
-      </c>
+        <v>4</v>
+      </c>
+      <c r="D27" t="inlineStr"/>
+      <c r="E27" t="inlineStr"/>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Friday</t>
+          <t>Thursday</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>8-11</t>
+          <t>23:00-02:00</t>
         </is>
       </c>
       <c r="C28" t="n">
-        <v>0</v>
-      </c>
-      <c r="D28" t="inlineStr">
-        <is>
-          <t>Thor Waguespack, Alejandro E. Ulvert, Noah Yaffe</t>
-        </is>
-      </c>
-      <c r="E28" t="inlineStr">
-        <is>
-          <t>Thor Waguespack, Alejandro E. Ulvert, Noah Yaffe</t>
-        </is>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="D28" t="inlineStr"/>
+      <c r="E28" t="inlineStr"/>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Friday</t>
+          <t>Thursday</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>11-2</t>
+          <t>02:00-08:00 (Night)</t>
         </is>
       </c>
       <c r="C29" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>Jack Mogelof, Ali Awada</t>
+          <t>Jaxon, Alejandro L</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>Jack Mogelof</t>
+          <t>Jaxon</t>
         </is>
       </c>
     </row>
@@ -1168,20 +1104,20 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>2-5</t>
+          <t>08:00-11:00</t>
         </is>
       </c>
       <c r="C30" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>Josh Greene, Henry, Adi</t>
+          <t>Ben Kairouz, Alexander, Blake Steel</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>Josh Greene, Adi</t>
+          <t>Ben Kairouz, Alexander, Blake Steel</t>
         </is>
       </c>
     </row>
@@ -1193,20 +1129,20 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>5-8</t>
+          <t>11:00-14:00</t>
         </is>
       </c>
       <c r="C31" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>Thor Waguespack, Blake Steel, Harry Corbin</t>
+          <t>Jamari Pitchford, George Ryckman, Jake Dieterich</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>Thor Waguespack, Blake Steel, Harry Corbin</t>
+          <t>Jamari Pitchford, George Ryckman</t>
         </is>
       </c>
     </row>
@@ -1218,20 +1154,20 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>8-11</t>
+          <t>14:00-17:00</t>
         </is>
       </c>
       <c r="C32" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>Josh Greene, Henry, George Ryckman</t>
+          <t>Kamsi, Paul, Alejandro Espinosa</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>Josh Greene, George Ryckman</t>
+          <t>Paul, Alejandro Espinosa</t>
         </is>
       </c>
     </row>
@@ -1243,20 +1179,20 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>11-2</t>
+          <t>17:00-20:00</t>
         </is>
       </c>
       <c r="C33" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>Alexander, Edu</t>
+          <t>Matheo, Noah Yaffe, Harry Corbin</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>Alexander, Edu</t>
+          <t>Matheo, Noah Yaffe, Harry Corbin</t>
         </is>
       </c>
     </row>
@@ -1268,70 +1204,54 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>2-8 (Night)</t>
+          <t>20:00-23:00</t>
         </is>
       </c>
       <c r="C34" t="n">
-        <v>6</v>
-      </c>
-      <c r="D34" t="inlineStr">
-        <is>
-          <t>Jaxon, Alejandro Espinosa</t>
-        </is>
-      </c>
-      <c r="E34" t="inlineStr">
-        <is>
-          <t>Jaxon, Alejandro Espinosa</t>
-        </is>
-      </c>
+        <v>4</v>
+      </c>
+      <c r="D34" t="inlineStr"/>
+      <c r="E34" t="inlineStr"/>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>Saturday</t>
+          <t>Friday</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>8-11</t>
+          <t>23:00-02:00</t>
         </is>
       </c>
       <c r="C35" t="n">
-        <v>0</v>
-      </c>
-      <c r="D35" t="inlineStr">
-        <is>
-          <t>Gabe Heller, Ezana, Harry Corbin</t>
-        </is>
-      </c>
-      <c r="E35" t="inlineStr">
-        <is>
-          <t>Gabe Heller, Harry Corbin</t>
-        </is>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="D35" t="inlineStr"/>
+      <c r="E35" t="inlineStr"/>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>Saturday</t>
+          <t>Friday</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>11-2</t>
+          <t>02:00-08:00 (Night)</t>
         </is>
       </c>
       <c r="C36" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>Jaxon, Ezana, Ali Awada</t>
+          <t>Ezana, Alejandro E. Ulvert</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>Jaxon</t>
+          <t>Alejandro E. Ulvert</t>
         </is>
       </c>
     </row>
@@ -1343,20 +1263,20 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>2-5</t>
+          <t>08:00-11:00</t>
         </is>
       </c>
       <c r="C37" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>Jaxon, Gabe Heller, Alexander</t>
+          <t>Kamsi, Josh Greene, Edu</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>Jaxon, Gabe Heller, Alexander</t>
+          <t>Josh Greene, Edu</t>
         </is>
       </c>
     </row>
@@ -1368,20 +1288,20 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>5-8</t>
+          <t>11:00-14:00</t>
         </is>
       </c>
       <c r="C38" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>Ben Kairouz, Alexander, Harry Corbin</t>
+          <t>Matheo, Alejandro L, Adi</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>Ben Kairouz, Alexander, Harry Corbin</t>
+          <t>Matheo, Adi</t>
         </is>
       </c>
     </row>
@@ -1393,20 +1313,20 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>8-11</t>
+          <t>14:00-17:00</t>
         </is>
       </c>
       <c r="C39" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>Alejandro L, George Ryckman, Blake Steel</t>
+          <t>Jack Mogelof, Thor Waguespack, Ali Awada</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>George Ryckman, Blake Steel</t>
+          <t>Jack Mogelof, Thor Waguespack</t>
         </is>
       </c>
     </row>
@@ -1418,20 +1338,20 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>11-2</t>
+          <t>17:00-20:00</t>
         </is>
       </c>
       <c r="C40" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>Ezana, Edu</t>
+          <t>Paul, Jamari Pitchford, Blake Steel</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>Edu</t>
+          <t>Paul, Jamari Pitchford, Blake Steel</t>
         </is>
       </c>
     </row>
@@ -1443,70 +1363,54 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>2-8 (Night)</t>
+          <t>20:00-23:00</t>
         </is>
       </c>
       <c r="C41" t="n">
-        <v>6</v>
-      </c>
-      <c r="D41" t="inlineStr">
-        <is>
-          <t>Henry, Jamari Pitchford</t>
-        </is>
-      </c>
-      <c r="E41" t="inlineStr">
-        <is>
-          <t>Jamari Pitchford</t>
-        </is>
-      </c>
+        <v>4</v>
+      </c>
+      <c r="D41" t="inlineStr"/>
+      <c r="E41" t="inlineStr"/>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>Sunday</t>
+          <t>Saturday</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>8-11</t>
+          <t>23:00-02:00</t>
         </is>
       </c>
       <c r="C42" t="n">
-        <v>0</v>
-      </c>
-      <c r="D42" t="inlineStr">
-        <is>
-          <t>Ben Kairouz, Kamsi, Paul</t>
-        </is>
-      </c>
-      <c r="E42" t="inlineStr">
-        <is>
-          <t>Ben Kairouz, Paul</t>
-        </is>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="D42" t="inlineStr"/>
+      <c r="E42" t="inlineStr"/>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>Sunday</t>
+          <t>Saturday</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>11-2</t>
+          <t>02:00-08:00 (Night)</t>
         </is>
       </c>
       <c r="C43" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>Jaxon, Jake Dieterich</t>
+          <t>Gabe Heller, Jake Dieterich</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>Jaxon</t>
+          <t>Gabe Heller</t>
         </is>
       </c>
     </row>
@@ -1518,20 +1422,20 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>2-5</t>
+          <t>08:00-11:00</t>
         </is>
       </c>
       <c r="C44" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>Jack Mogelof, Josh Greene, Jake Dieterich</t>
+          <t>Jack Mogelof, Henry, George Ryckman</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>Jack Mogelof, Josh Greene</t>
+          <t>Jack Mogelof, George Ryckman</t>
         </is>
       </c>
     </row>
@@ -1543,20 +1447,20 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>8-11</t>
+          <t>11:00-14:00</t>
         </is>
       </c>
       <c r="C45" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>Paul, Matheo, Noah Yaffe</t>
+          <t>Ben Kairouz, Alejandro L, Adi</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>Paul, Matheo, Noah Yaffe</t>
+          <t>Ben Kairouz, Adi</t>
         </is>
       </c>
     </row>
@@ -1568,20 +1472,20 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>11-2</t>
+          <t>14:00-17:00</t>
         </is>
       </c>
       <c r="C46" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>Ben Kairouz, Ezana</t>
+          <t>Alexander, Noah Yaffe, Harry Corbin</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>Ben Kairouz</t>
+          <t>Alexander, Noah Yaffe, Harry Corbin</t>
         </is>
       </c>
     </row>
@@ -1593,20 +1497,71 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>2-8 (Night)</t>
+          <t>17:00-20:00</t>
         </is>
       </c>
       <c r="C47" t="n">
+        <v>3</v>
+      </c>
+      <c r="D47" t="inlineStr"/>
+      <c r="E47" t="inlineStr"/>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>Sunday</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>20:00-23:00</t>
+        </is>
+      </c>
+      <c r="C48" t="n">
+        <v>4</v>
+      </c>
+      <c r="D48" t="inlineStr"/>
+      <c r="E48" t="inlineStr"/>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>Sunday</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>23:00-02:00</t>
+        </is>
+      </c>
+      <c r="C49" t="n">
         <v>5</v>
       </c>
-      <c r="D47" t="inlineStr">
-        <is>
-          <t>Ben Kairouz, Alejandro E. Ulvert</t>
-        </is>
-      </c>
-      <c r="E47" t="inlineStr">
-        <is>
-          <t>Ben Kairouz, Alejandro E. Ulvert</t>
+      <c r="D49" t="inlineStr"/>
+      <c r="E49" t="inlineStr"/>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>Sunday</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>02:00-08:00 (Night)</t>
+        </is>
+      </c>
+      <c r="C50" t="n">
+        <v>6</v>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>Alejandro Espinosa, Edu</t>
+        </is>
+      </c>
+      <c r="E50" t="inlineStr">
+        <is>
+          <t>Alejandro Espinosa, Edu</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Remove CSV conversion utility and update schedule output format
</commit_message>
<xml_diff>
--- a/schedule_output.xlsx
+++ b/schedule_output.xlsx
@@ -476,12 +476,12 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Alexander, Alejandro L, Adi</t>
+          <t>Paul, Thor Waguespack, Alejandro E. Ulvert</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Alexander, Adi</t>
+          <t>Paul, Thor Waguespack, Alejandro E. Ulvert</t>
         </is>
       </c>
     </row>
@@ -501,12 +501,12 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Jaxon, Ben Kairouz, Kamsi</t>
+          <t>Ben Kairouz, Alexander, Jamari Pitchford</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Jaxon, Ben Kairouz</t>
+          <t>Ben Kairouz, Alexander, Jamari Pitchford</t>
         </is>
       </c>
     </row>
@@ -526,12 +526,12 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Henry, Jamari Pitchford, Harry Corbin</t>
+          <t>Jaxon, Alejandro Espinosa, George Ryckman</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Jamari Pitchford, Harry Corbin</t>
+          <t>Jaxon, Alejandro Espinosa, George Ryckman</t>
         </is>
       </c>
     </row>
@@ -551,12 +551,12 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Thor Waguespack, Ali Awada, Alejandro E. Ulvert</t>
+          <t>Jack Mogelof, Jake Dieterich, Adi</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Thor Waguespack, Alejandro E. Ulvert</t>
+          <t>Jack Mogelof, Adi</t>
         </is>
       </c>
     </row>
@@ -574,8 +574,16 @@
       <c r="C6" t="n">
         <v>4</v>
       </c>
-      <c r="D6" t="inlineStr"/>
-      <c r="E6" t="inlineStr"/>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Gabe Heller, Alejandro L</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>Gabe Heller</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -591,7 +599,11 @@
       <c r="C7" t="n">
         <v>5</v>
       </c>
-      <c r="D7" t="inlineStr"/>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>Henry</t>
+        </is>
+      </c>
       <c r="E7" t="inlineStr"/>
     </row>
     <row r="8">
@@ -610,12 +622,12 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Ezana, Paul</t>
+          <t>Noah Yaffe</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>Paul</t>
+          <t>Noah Yaffe</t>
         </is>
       </c>
     </row>
@@ -635,12 +647,12 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Paul, Alexander, George Ryckman</t>
+          <t>Jack Mogelof, Jake Dieterich, Adi</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>Paul, Alexander, George Ryckman</t>
+          <t>Jack Mogelof, Adi</t>
         </is>
       </c>
     </row>
@@ -660,12 +672,12 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Alejandro Espinosa, Jamari Pitchford, Blake Steel</t>
+          <t>Ben Kairouz, Paul, Alejandro Espinosa</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>Alejandro Espinosa, Jamari Pitchford, Blake Steel</t>
+          <t>Ben Kairouz, Paul, Alejandro Espinosa</t>
         </is>
       </c>
     </row>
@@ -685,12 +697,12 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Josh Greene, Matheo, Jake Dieterich</t>
+          <t>Ezana, Edu, Blake Steel</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>Josh Greene, Matheo</t>
+          <t>Edu, Blake Steel</t>
         </is>
       </c>
     </row>
@@ -710,12 +722,12 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>Jaxon, Gabe Heller, Alejandro E. Ulvert</t>
+          <t>Alexander, Jamari Pitchford, George Ryckman</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>Jaxon, Gabe Heller, Alejandro E. Ulvert</t>
+          <t>Alexander, Jamari Pitchford, George Ryckman</t>
         </is>
       </c>
     </row>
@@ -750,7 +762,11 @@
       <c r="C14" t="n">
         <v>5</v>
       </c>
-      <c r="D14" t="inlineStr"/>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>Henry</t>
+        </is>
+      </c>
       <c r="E14" t="inlineStr"/>
     </row>
     <row r="15">
@@ -767,16 +783,8 @@
       <c r="C15" t="n">
         <v>6</v>
       </c>
-      <c r="D15" t="inlineStr">
-        <is>
-          <t>Jack Mogelof, Henry</t>
-        </is>
-      </c>
-      <c r="E15" t="inlineStr">
-        <is>
-          <t>Jack Mogelof</t>
-        </is>
-      </c>
+      <c r="D15" t="inlineStr"/>
+      <c r="E15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -794,12 +802,12 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>Ezana, Josh Greene, Thor Waguespack</t>
+          <t>Matheo, Alejandro L, Noah Yaffe</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>Josh Greene, Thor Waguespack</t>
+          <t>Matheo, Noah Yaffe</t>
         </is>
       </c>
     </row>
@@ -819,12 +827,12 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>Gabe Heller, Jake Dieterich, Noah Yaffe</t>
+          <t>Gabe Heller, Ben Kairouz, Thor Waguespack</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>Gabe Heller, Noah Yaffe</t>
+          <t>Gabe Heller, Ben Kairouz, Thor Waguespack</t>
         </is>
       </c>
     </row>
@@ -844,12 +852,12 @@
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>Henry, Alejandro Espinosa, Edu</t>
+          <t>Jaxon, Kamsi, Josh Greene</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>Alejandro Espinosa, Edu</t>
+          <t>Jaxon, Josh Greene</t>
         </is>
       </c>
     </row>
@@ -869,12 +877,12 @@
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>Ben Kairouz, Kamsi, Harry Corbin</t>
+          <t>Edu, Ali Awada, Harry Corbin</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>Ben Kairouz, Harry Corbin</t>
+          <t>Edu, Harry Corbin</t>
         </is>
       </c>
     </row>
@@ -892,8 +900,16 @@
       <c r="C20" t="n">
         <v>4</v>
       </c>
-      <c r="D20" t="inlineStr"/>
-      <c r="E20" t="inlineStr"/>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>Ezana, Blake Steel</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>Blake Steel</t>
+        </is>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -928,14 +944,10 @@
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>Ali Awada, Blake Steel</t>
-        </is>
-      </c>
-      <c r="E22" t="inlineStr">
-        <is>
-          <t>Blake Steel</t>
-        </is>
-      </c>
+          <t>Henry</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr"/>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -953,12 +965,12 @@
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>Jack Mogelof, George Ryckman, Noah Yaffe</t>
+          <t>Kamsi, Josh Greene, Matheo</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>Jack Mogelof, George Ryckman, Noah Yaffe</t>
+          <t>Josh Greene, Matheo</t>
         </is>
       </c>
     </row>
@@ -978,12 +990,12 @@
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>Ezana, Josh Greene, Thor Waguespack</t>
+          <t>Paul, Jamari Pitchford, Thor Waguespack</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>Josh Greene, Thor Waguespack</t>
+          <t>Paul, Jamari Pitchford, Thor Waguespack</t>
         </is>
       </c>
     </row>
@@ -1003,12 +1015,12 @@
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>Gabe Heller, Ali Awada, Alejandro E. Ulvert</t>
+          <t>Gabe Heller, Ezana, Blake Steel</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>Gabe Heller, Alejandro E. Ulvert</t>
+          <t>Gabe Heller, Blake Steel</t>
         </is>
       </c>
     </row>
@@ -1028,12 +1040,12 @@
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>Matheo, Edu, Adi</t>
+          <t>Jack Mogelof, George Ryckman, Alejandro E. Ulvert</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>Matheo, Edu, Adi</t>
+          <t>Jack Mogelof, George Ryckman, Alejandro E. Ulvert</t>
         </is>
       </c>
     </row>
@@ -1068,7 +1080,11 @@
       <c r="C28" t="n">
         <v>5</v>
       </c>
-      <c r="D28" t="inlineStr"/>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>Henry</t>
+        </is>
+      </c>
       <c r="E28" t="inlineStr"/>
     </row>
     <row r="29">
@@ -1085,16 +1101,8 @@
       <c r="C29" t="n">
         <v>6</v>
       </c>
-      <c r="D29" t="inlineStr">
-        <is>
-          <t>Jaxon, Alejandro L</t>
-        </is>
-      </c>
-      <c r="E29" t="inlineStr">
-        <is>
-          <t>Jaxon</t>
-        </is>
-      </c>
+      <c r="D29" t="inlineStr"/>
+      <c r="E29" t="inlineStr"/>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -1112,12 +1120,12 @@
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>Ben Kairouz, Alexander, Blake Steel</t>
+          <t>Jaxon, Jake Dieterich, Alejandro E. Ulvert</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>Ben Kairouz, Alexander, Blake Steel</t>
+          <t>Jaxon, Alejandro E. Ulvert</t>
         </is>
       </c>
     </row>
@@ -1137,12 +1145,12 @@
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>Jamari Pitchford, George Ryckman, Jake Dieterich</t>
+          <t>Jamari Pitchford, Thor Waguespack, Ali Awada</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>Jamari Pitchford, George Ryckman</t>
+          <t>Jamari Pitchford, Thor Waguespack</t>
         </is>
       </c>
     </row>
@@ -1162,12 +1170,12 @@
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>Kamsi, Paul, Alejandro Espinosa</t>
+          <t>Ben Kairouz, George Ryckman, Adi</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>Paul, Alejandro Espinosa</t>
+          <t>Ben Kairouz, George Ryckman, Adi</t>
         </is>
       </c>
     </row>
@@ -1187,12 +1195,12 @@
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>Matheo, Noah Yaffe, Harry Corbin</t>
+          <t>Jack Mogelof, Alejandro Espinosa, Harry Corbin</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>Matheo, Noah Yaffe, Harry Corbin</t>
+          <t>Jack Mogelof, Alejandro Espinosa, Harry Corbin</t>
         </is>
       </c>
     </row>
@@ -1227,7 +1235,11 @@
       <c r="C35" t="n">
         <v>5</v>
       </c>
-      <c r="D35" t="inlineStr"/>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>Kamsi</t>
+        </is>
+      </c>
       <c r="E35" t="inlineStr"/>
     </row>
     <row r="36">
@@ -1244,16 +1256,8 @@
       <c r="C36" t="n">
         <v>6</v>
       </c>
-      <c r="D36" t="inlineStr">
-        <is>
-          <t>Ezana, Alejandro E. Ulvert</t>
-        </is>
-      </c>
-      <c r="E36" t="inlineStr">
-        <is>
-          <t>Alejandro E. Ulvert</t>
-        </is>
-      </c>
+      <c r="D36" t="inlineStr"/>
+      <c r="E36" t="inlineStr"/>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
@@ -1271,12 +1275,12 @@
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>Kamsi, Josh Greene, Edu</t>
+          <t>Josh Greene, Adi, Harry Corbin</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>Josh Greene, Edu</t>
+          <t>Josh Greene, Adi, Harry Corbin</t>
         </is>
       </c>
     </row>
@@ -1296,12 +1300,12 @@
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>Matheo, Alejandro L, Adi</t>
+          <t>Jaxon, Paul, Alejandro L</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>Matheo, Adi</t>
+          <t>Jaxon, Paul</t>
         </is>
       </c>
     </row>
@@ -1321,12 +1325,12 @@
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>Jack Mogelof, Thor Waguespack, Ali Awada</t>
+          <t>Alexander, Edu, Jake Dieterich</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>Jack Mogelof, Thor Waguespack</t>
+          <t>Alexander, Edu</t>
         </is>
       </c>
     </row>
@@ -1346,12 +1350,12 @@
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>Paul, Jamari Pitchford, Blake Steel</t>
+          <t>Alejandro Espinosa, Ali Awada, Alejandro E. Ulvert</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>Paul, Jamari Pitchford, Blake Steel</t>
+          <t>Alejandro Espinosa, Alejandro E. Ulvert</t>
         </is>
       </c>
     </row>
@@ -1405,12 +1409,12 @@
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>Gabe Heller, Jake Dieterich</t>
+          <t>Matheo, Noah Yaffe</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>Gabe Heller</t>
+          <t>Matheo, Noah Yaffe</t>
         </is>
       </c>
     </row>
@@ -1430,12 +1434,12 @@
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>Jack Mogelof, Henry, George Ryckman</t>
+          <t>Josh Greene, Alejandro L, Harry Corbin</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>Jack Mogelof, George Ryckman</t>
+          <t>Josh Greene, Harry Corbin</t>
         </is>
       </c>
     </row>
@@ -1455,12 +1459,12 @@
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>Ben Kairouz, Alejandro L, Adi</t>
+          <t>Ezana, Alexander, Edu</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>Ben Kairouz, Adi</t>
+          <t>Alexander, Edu</t>
         </is>
       </c>
     </row>
@@ -1480,12 +1484,12 @@
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>Alexander, Noah Yaffe, Harry Corbin</t>
+          <t>Gabe Heller, Ali Awada, Noah Yaffe</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>Alexander, Noah Yaffe, Harry Corbin</t>
+          <t>Gabe Heller, Noah Yaffe</t>
         </is>
       </c>
     </row>
@@ -1503,8 +1507,16 @@
       <c r="C47" t="n">
         <v>3</v>
       </c>
-      <c r="D47" t="inlineStr"/>
-      <c r="E47" t="inlineStr"/>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>Kamsi, Blake Steel</t>
+        </is>
+      </c>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>Blake Steel</t>
+        </is>
+      </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
@@ -1520,8 +1532,16 @@
       <c r="C48" t="n">
         <v>4</v>
       </c>
-      <c r="D48" t="inlineStr"/>
-      <c r="E48" t="inlineStr"/>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>Matheo</t>
+        </is>
+      </c>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>Matheo</t>
+        </is>
+      </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
@@ -1554,16 +1574,8 @@
       <c r="C50" t="n">
         <v>6</v>
       </c>
-      <c r="D50" t="inlineStr">
-        <is>
-          <t>Alejandro Espinosa, Edu</t>
-        </is>
-      </c>
-      <c r="E50" t="inlineStr">
-        <is>
-          <t>Alejandro Espinosa, Edu</t>
-        </is>
-      </c>
+      <c r="D50" t="inlineStr"/>
+      <c r="E50" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>